<commit_message>
Some test execel files, expereiments
</commit_message>
<xml_diff>
--- a/data/test_input.xlsx
+++ b/data/test_input.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://columbusglobal-my.sharepoint.com/personal/voev_columbusglobal_com/Documents/av_doc/Vehicle-Routing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{1C197FCC-D555-4110-9B11-7FD88CA513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4316D6DF-B4A5-4A02-A176-09D95997D74A}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{1C197FCC-D555-4110-9B11-7FD88CA513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{723B9F6F-E37C-4415-A002-D3264A6A9504}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="0" windowWidth="21732" windowHeight="11700" activeTab="4" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
+    <workbookView xWindow="96" yWindow="300" windowWidth="21732" windowHeight="11700" activeTab="4" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Cities" sheetId="2" r:id="rId2"/>
-    <sheet name="Cars" sheetId="3" r:id="rId3"/>
-    <sheet name="Orders" sheetId="4" r:id="rId4"/>
-    <sheet name="SimpleOrders" sheetId="6" r:id="rId5"/>
-    <sheet name="Routes" sheetId="5" r:id="rId6"/>
+    <sheet name="Vehicles" sheetId="3" r:id="rId3"/>
+    <sheet name="Orders" sheetId="6" r:id="rId4"/>
+    <sheet name="Routes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>minPeriod</t>
   </si>
@@ -605,150 +604,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FCF74F2-5841-483E-B084-25638E0734F9}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>150</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>150</v>
-      </c>
-      <c r="D4">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCA095E-D3F7-49C8-BD5C-B9B8E0BE66A7}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
@@ -822,11 +681,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723586A4-2014-4229-857C-3037F57FC317}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>